<commit_message>
updated links and more
</commit_message>
<xml_diff>
--- a/cv_zmm.xlsx
+++ b/cv_zmm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecc85ccb002dd88c/Resumes/Git-Hub/Website/zacharymilosmoore/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="8_{4CB44A4F-E1F1-4138-AC98-038A281BC4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A36F78BC-FFEB-4D7A-95E4-9DB34762A0A5}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="8_{4CB44A4F-E1F1-4138-AC98-038A281BC4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00D23A6C-C9BD-41AA-BF46-ACB5B0A9ECB9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4154936E-D054-4D45-B3AE-FD317E846EC6}"/>
   </bookViews>
@@ -1956,9 +1956,6 @@
     <t xml:space="preserve">Awarded in competition of 10 undergraduate students for poster presentation on connecting life history traits and community dynamics. </t>
   </si>
   <si>
-    <t>www.umanitoba.ca</t>
-  </si>
-  <si>
     <t>Org_Link</t>
   </si>
   <si>
@@ -2176,6 +2173,9 @@
   </si>
   <si>
     <t xml:space="preserve">Learned to liase with land managers. Excelled in communicating complex issues to varied audiences. </t>
+  </si>
+  <si>
+    <t>https://www.umanitoba.ca/</t>
   </si>
 </sst>
 </file>
@@ -2493,116 +2493,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="87">
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;Present&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;Present&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;Present&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;Present&quot;"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3334,6 +3224,74 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3996,6 +3954,48 @@
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;Present&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;Present&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;Present&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;Present&quot;"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4010,18 +4010,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E6C429B5-94AF-4DF8-8EEB-230783D5C112}" name="cv.table" displayName="cv.table" ref="A1:AK69" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E6C429B5-94AF-4DF8-8EEB-230783D5C112}" name="cv.table" displayName="cv.table" ref="A1:AK69" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <autoFilter ref="A1:AK69" xr:uid="{51C5574A-10F4-4984-BAF7-4488D8AC8419}">
     <filterColumn colId="2">
       <filters>
         <filter val="Education"/>
         <filter val="Employment"/>
         <filter val="Projects"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Nature Conservancy Canada"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4032,97 +4027,97 @@
     <sortCondition descending="1" ref="J2:J69"/>
   </sortState>
   <tableColumns count="37">
-    <tableColumn id="26" xr3:uid="{9B11C92F-E956-4444-BEFF-953F753416F5}" name="CV" dataDxfId="84"/>
-    <tableColumn id="11" xr3:uid="{34502BA5-FB1E-4B40-8788-421DADDD3E97}" name="Branch" dataDxfId="83"/>
-    <tableColumn id="1" xr3:uid="{70612BCC-1448-430F-9D24-28D063F5A2A3}" name="Category" dataDxfId="82"/>
-    <tableColumn id="18" xr3:uid="{5E4EDA0C-2B9B-42CE-A32B-4403948C8E7B}" name="Type" dataDxfId="81"/>
-    <tableColumn id="7" xr3:uid="{EC86C6DE-554D-4F33-AEC2-DF6E1CA6068F}" name="Organization" dataDxfId="80"/>
-    <tableColumn id="24" xr3:uid="{2E4ADD2D-C302-4284-95AA-617479194CFD}" name="Org_Link" dataDxfId="79"/>
-    <tableColumn id="8" xr3:uid="{26CD9B61-38AB-4312-B98A-E2A336BF9AB7}" name="Org_Acr" dataDxfId="78"/>
-    <tableColumn id="9" xr3:uid="{2BE7F400-F53C-40A9-BB7D-530918FE5571}" name="Title" dataDxfId="77"/>
-    <tableColumn id="10" xr3:uid="{33E88F9D-A2A0-44DD-84D2-308042D95210}" name="Pos_Acr" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{6738E286-0938-42F9-B68F-D49892936B3D}" name="Start" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{F83278BD-725D-4108-95A1-F217E27DC898}" name="End" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{802621DE-7866-4555-8E12-DD03949FA7E7}" name="Start_Month" dataDxfId="73">
+    <tableColumn id="26" xr3:uid="{9B11C92F-E956-4444-BEFF-953F753416F5}" name="CV" dataDxfId="78"/>
+    <tableColumn id="11" xr3:uid="{34502BA5-FB1E-4B40-8788-421DADDD3E97}" name="Branch" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{70612BCC-1448-430F-9D24-28D063F5A2A3}" name="Category" dataDxfId="76"/>
+    <tableColumn id="18" xr3:uid="{5E4EDA0C-2B9B-42CE-A32B-4403948C8E7B}" name="Type" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{EC86C6DE-554D-4F33-AEC2-DF6E1CA6068F}" name="Organization" dataDxfId="74"/>
+    <tableColumn id="24" xr3:uid="{2E4ADD2D-C302-4284-95AA-617479194CFD}" name="Org_Link" dataDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{26CD9B61-38AB-4312-B98A-E2A336BF9AB7}" name="Org_Acr" dataDxfId="72"/>
+    <tableColumn id="9" xr3:uid="{2BE7F400-F53C-40A9-BB7D-530918FE5571}" name="Title" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{33E88F9D-A2A0-44DD-84D2-308042D95210}" name="Pos_Acr" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{6738E286-0938-42F9-B68F-D49892936B3D}" name="Start" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{F83278BD-725D-4108-95A1-F217E27DC898}" name="End" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{802621DE-7866-4555-8E12-DD03949FA7E7}" name="Start_Month" dataDxfId="67">
       <calculatedColumnFormula>MONTH(cv.table[[#This Row],[Start]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{C6566D99-33F8-4C29-9F77-57CB96E0A79F}" name="Start_Year" dataDxfId="72">
+    <tableColumn id="20" xr3:uid="{C6566D99-33F8-4C29-9F77-57CB96E0A79F}" name="Start_Year" dataDxfId="66">
       <calculatedColumnFormula>YEAR(cv.table[[#This Row],[Start]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{6BF152A0-7851-42D9-985D-3CC266F2660D}" name="End_Month" dataDxfId="71">
+    <tableColumn id="22" xr3:uid="{6BF152A0-7851-42D9-985D-3CC266F2660D}" name="End_Month" dataDxfId="65">
       <calculatedColumnFormula>MONTH(cv.table[[#This Row],[End]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{FEEC95E2-B833-448E-AC76-6DBAE4E45591}" name="End_Year" dataDxfId="70">
+    <tableColumn id="21" xr3:uid="{FEEC95E2-B833-448E-AC76-6DBAE4E45591}" name="End_Year" dataDxfId="64">
       <calculatedColumnFormula>YEAR(cv.table[[#This Row],[End]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7BB222DF-5EE2-4BC9-9EF1-E1A53AFE31F4}" name="Time" dataDxfId="69">
+    <tableColumn id="5" xr3:uid="{7BB222DF-5EE2-4BC9-9EF1-E1A53AFE31F4}" name="Time" dataDxfId="63">
       <calculatedColumnFormula>IF((Q2="Days"),((K2-J2+1)),IF(Q2="Months",((K2-J2)/30),((K2-J2)/365)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{436D180E-D520-4622-BF48-C117C2F3D72D}" name="Time_Unit" dataDxfId="68"/>
-    <tableColumn id="14" xr3:uid="{0AC0D461-4004-4A64-B5A7-5BCBB135C7C9}" name="Loc_Small" dataDxfId="67"/>
-    <tableColumn id="15" xr3:uid="{604F7BAB-42A3-455E-8C18-202B68AEBC37}" name="Loc_Large" dataDxfId="66"/>
-    <tableColumn id="12" xr3:uid="{1CAEFFF7-88CF-4AB8-88EF-1DC65D78A14C}" name="Description" dataDxfId="65"/>
-    <tableColumn id="19" xr3:uid="{B4A2DCCB-9505-42D1-97AE-1B44581F30F1}" name="Tasks" dataDxfId="64"/>
-    <tableColumn id="16" xr3:uid="{9AA8F708-1C30-48AB-8EDD-8C5BF442D6ED}" name="Lessons" dataDxfId="63"/>
-    <tableColumn id="17" xr3:uid="{CAB8C078-3C62-4846-9AC3-0B17AD693416}" name="Achievements" dataDxfId="62"/>
-    <tableColumn id="13" xr3:uid="{982B9A83-407B-47DD-AE12-B9AF5B9B6C73}" name="Notes" dataDxfId="61"/>
-    <tableColumn id="23" xr3:uid="{4C96C715-152C-4914-BB38-FEFF25E58297}" name="V1" dataDxfId="60"/>
-    <tableColumn id="25" xr3:uid="{AB48772A-9139-4A74-BF34-9532AF007D28}" name="V1_Desc" dataDxfId="59"/>
-    <tableColumn id="31" xr3:uid="{ABB7B8F1-D658-471C-B518-50B31EDEA024}" name="V1_Type" dataDxfId="58"/>
-    <tableColumn id="27" xr3:uid="{AA368EEC-19E0-4A9A-90A5-B309B7AE3A50}" name="V2" dataDxfId="57"/>
-    <tableColumn id="28" xr3:uid="{65DF71FF-E9EE-4AAB-A467-1B0F813F20A6}" name="V2_Desc" dataDxfId="56"/>
-    <tableColumn id="29" xr3:uid="{C2677FEE-8349-4A02-B596-66E45AD44952}" name="V3" dataDxfId="55"/>
-    <tableColumn id="30" xr3:uid="{1E758BB4-3C89-4653-80DA-C549531B5244}" name="V3_Desc" dataDxfId="54"/>
-    <tableColumn id="32" xr3:uid="{FEE44D7E-69A0-4B71-AB66-1461C45267FF}" name="L1" dataDxfId="53"/>
-    <tableColumn id="33" xr3:uid="{21C268AA-32E8-4627-82E0-7A62468157B5}" name="L1_Desc" dataDxfId="52"/>
-    <tableColumn id="34" xr3:uid="{E85C2701-53A9-4B93-B733-9B7CD3138938}" name="L2" dataDxfId="51"/>
-    <tableColumn id="35" xr3:uid="{8E33C990-20D6-41EA-81EB-AF8C09425D76}" name="L2_Desc" dataDxfId="50"/>
-    <tableColumn id="36" xr3:uid="{FF798E68-0DB4-421A-AE12-25569247C412}" name="L3" dataDxfId="49"/>
-    <tableColumn id="37" xr3:uid="{BF4D3938-CF08-433F-8B81-A515F3E1BBB7}" name="L3_Desc" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{436D180E-D520-4622-BF48-C117C2F3D72D}" name="Time_Unit" dataDxfId="62"/>
+    <tableColumn id="14" xr3:uid="{0AC0D461-4004-4A64-B5A7-5BCBB135C7C9}" name="Loc_Small" dataDxfId="61"/>
+    <tableColumn id="15" xr3:uid="{604F7BAB-42A3-455E-8C18-202B68AEBC37}" name="Loc_Large" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{1CAEFFF7-88CF-4AB8-88EF-1DC65D78A14C}" name="Description" dataDxfId="59"/>
+    <tableColumn id="19" xr3:uid="{B4A2DCCB-9505-42D1-97AE-1B44581F30F1}" name="Tasks" dataDxfId="58"/>
+    <tableColumn id="16" xr3:uid="{9AA8F708-1C30-48AB-8EDD-8C5BF442D6ED}" name="Lessons" dataDxfId="57"/>
+    <tableColumn id="17" xr3:uid="{CAB8C078-3C62-4846-9AC3-0B17AD693416}" name="Achievements" dataDxfId="56"/>
+    <tableColumn id="13" xr3:uid="{982B9A83-407B-47DD-AE12-B9AF5B9B6C73}" name="Notes" dataDxfId="55"/>
+    <tableColumn id="23" xr3:uid="{4C96C715-152C-4914-BB38-FEFF25E58297}" name="V1" dataDxfId="54"/>
+    <tableColumn id="25" xr3:uid="{AB48772A-9139-4A74-BF34-9532AF007D28}" name="V1_Desc" dataDxfId="53"/>
+    <tableColumn id="31" xr3:uid="{ABB7B8F1-D658-471C-B518-50B31EDEA024}" name="V1_Type" dataDxfId="52"/>
+    <tableColumn id="27" xr3:uid="{AA368EEC-19E0-4A9A-90A5-B309B7AE3A50}" name="V2" dataDxfId="51"/>
+    <tableColumn id="28" xr3:uid="{65DF71FF-E9EE-4AAB-A467-1B0F813F20A6}" name="V2_Desc" dataDxfId="50"/>
+    <tableColumn id="29" xr3:uid="{C2677FEE-8349-4A02-B596-66E45AD44952}" name="V3" dataDxfId="49"/>
+    <tableColumn id="30" xr3:uid="{1E758BB4-3C89-4653-80DA-C549531B5244}" name="V3_Desc" dataDxfId="48"/>
+    <tableColumn id="32" xr3:uid="{FEE44D7E-69A0-4B71-AB66-1461C45267FF}" name="L1" dataDxfId="47"/>
+    <tableColumn id="33" xr3:uid="{21C268AA-32E8-4627-82E0-7A62468157B5}" name="L1_Desc" dataDxfId="46"/>
+    <tableColumn id="34" xr3:uid="{E85C2701-53A9-4B93-B733-9B7CD3138938}" name="L2" dataDxfId="45"/>
+    <tableColumn id="35" xr3:uid="{8E33C990-20D6-41EA-81EB-AF8C09425D76}" name="L2_Desc" dataDxfId="44"/>
+    <tableColumn id="36" xr3:uid="{FF798E68-0DB4-421A-AE12-25569247C412}" name="L3" dataDxfId="43"/>
+    <tableColumn id="37" xr3:uid="{BF4D3938-CF08-433F-8B81-A515F3E1BBB7}" name="L3_Desc" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B570B70E-C899-455A-AC26-A13A5D4A9E92}" name="Applications" displayName="Applications" ref="A1:N49" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B570B70E-C899-455A-AC26-A13A5D4A9E92}" name="Applications" displayName="Applications" ref="A1:N49" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:N49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
-    <tableColumn id="12" xr3:uid="{218087FE-17C0-423E-B6F8-901859622287}" name="Stage" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{D9613474-92D2-4050-ACF2-B118452426A7}" name="Period" dataDxfId="44"/>
-    <tableColumn id="1" xr3:uid="{5BAA014C-1241-4434-8AD7-745DA50962BB}" name="Application.Date" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{983FF83C-F5E6-4F96-A5C4-E0DE49B59CF1}" name="Closing.Date" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{B6DA3B76-2EA9-477C-916B-C85ABE14EDEA}" name="Organization" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{F810C504-FE42-4544-B62D-AD9215CC2056}" name="Role" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{9092FFA8-86C9-4C39-B086-D49B5605E883}" name="Location" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{82ADB252-CBD3-45E3-93DC-F3E245711EE6}" name="Length" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{D67F4400-95EC-4574-AC0A-5E80B43AE8EA}" name="Pay" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{61429A75-040E-4A75-9265-393C74FD1D63}" name="Contact" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{7F27D872-9FAA-49C7-AD85-D69344560AD6}" name="Title" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{F6EC3991-C4AE-4478-9730-0BDA10018440}" name="Contact.Information" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{64723C84-D17F-4973-A41F-D234D9E037AB}" name="Format" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{C898DE17-6DCD-4913-9793-AC56DC7DDFBB}" name="Notes" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{218087FE-17C0-423E-B6F8-901859622287}" name="Stage" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{D9613474-92D2-4050-ACF2-B118452426A7}" name="Period" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{5BAA014C-1241-4434-8AD7-745DA50962BB}" name="Application.Date" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{983FF83C-F5E6-4F96-A5C4-E0DE49B59CF1}" name="Closing.Date" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{B6DA3B76-2EA9-477C-916B-C85ABE14EDEA}" name="Organization" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{F810C504-FE42-4544-B62D-AD9215CC2056}" name="Role" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{9092FFA8-86C9-4C39-B086-D49B5605E883}" name="Location" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{82ADB252-CBD3-45E3-93DC-F3E245711EE6}" name="Length" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{D67F4400-95EC-4574-AC0A-5E80B43AE8EA}" name="Pay" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{61429A75-040E-4A75-9265-393C74FD1D63}" name="Contact" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{7F27D872-9FAA-49C7-AD85-D69344560AD6}" name="Title" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{F6EC3991-C4AE-4478-9730-0BDA10018440}" name="Contact.Information" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{64723C84-D17F-4973-A41F-D234D9E037AB}" name="Format" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{C898DE17-6DCD-4913-9793-AC56DC7DDFBB}" name="Notes" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A7031F1-2203-44EF-8965-9D3E7E6E20C7}" name="Lists" displayName="Lists" ref="A1:L10" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A7031F1-2203-44EF-8965-9D3E7E6E20C7}" name="Lists" displayName="Lists" ref="A1:L10" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:L10" xr:uid="{F02DA2C5-59F4-4989-BB36-1611149FB962}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{308CFDE8-BE03-456B-84E3-E26E079B0F80}" name="Branch" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{4D4C6EDC-3308-4CFE-89F0-A12C8F5152D6}" name="Category" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{F8982A44-14CE-484F-B8CB-BB3EC9A5ED07}" name="Accreditation" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{6D21A9C5-BEA7-476E-A983-243C0B9BEC34}" name="Award" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{C1A44E26-D96B-4ADC-A0DE-C7DE9818C883}" name="Certificate" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{5878EC92-DA44-448C-8DFE-354AB46F1B50}" name="Event" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{B8C94F22-10CD-4485-A36C-EF94EFB8544F}" name="Education" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{36320B06-26D8-4E21-A082-28EFC253ECC4}" name="Employment" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{EF5D7AD2-86C4-4842-A36A-B12726CEFC56}" name="Membership" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{F05A780B-4496-4C27-9705-F129B2480E2D}" name="Project" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{8FF5F1B6-1539-487D-A296-90D274FBA601}" name="Volunteering" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{932C090C-7AD8-4B1D-90AE-36BA3B8B76F8}" name="Application.Stage" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{308CFDE8-BE03-456B-84E3-E26E079B0F80}" name="Branch" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4D4C6EDC-3308-4CFE-89F0-A12C8F5152D6}" name="Category" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{F8982A44-14CE-484F-B8CB-BB3EC9A5ED07}" name="Accreditation" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{6D21A9C5-BEA7-476E-A983-243C0B9BEC34}" name="Award" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{C1A44E26-D96B-4ADC-A0DE-C7DE9818C883}" name="Certificate" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{5878EC92-DA44-448C-8DFE-354AB46F1B50}" name="Event" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{B8C94F22-10CD-4485-A36C-EF94EFB8544F}" name="Education" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{36320B06-26D8-4E21-A082-28EFC253ECC4}" name="Employment" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{EF5D7AD2-86C4-4842-A36A-B12726CEFC56}" name="Membership" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{F05A780B-4496-4C27-9705-F129B2480E2D}" name="Project" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{8FF5F1B6-1539-487D-A296-90D274FBA601}" name="Volunteering" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{932C090C-7AD8-4B1D-90AE-36BA3B8B76F8}" name="Application.Stage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4444,8 +4439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6961E3D5-6E55-490E-8BC2-FDE92C6153D9}">
   <dimension ref="A1:AK69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4493,7 +4488,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>24</v>
@@ -4550,46 +4545,46 @@
         <v>10</v>
       </c>
       <c r="Y1" s="8" t="s">
+        <v>633</v>
+      </c>
+      <c r="Z1" s="8" t="s">
         <v>634</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="AB1" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="AA1" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>637</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="AE1" s="8" t="s">
-        <v>639</v>
-      </c>
       <c r="AF1" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="AG1" s="8" t="s">
         <v>646</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>649</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AK1" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="AK1" s="8" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>477</v>
       </c>
@@ -4606,7 +4601,7 @@
         <v>440</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>630</v>
+        <v>703</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>441</v>
@@ -4653,7 +4648,7 @@
         <v>446</v>
       </c>
       <c r="T2" s="39" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="U2" s="39"/>
       <c r="V2" s="39"/>
@@ -4675,7 +4670,7 @@
       <c r="AJ2" s="39"/>
       <c r="AK2" s="39"/>
     </row>
-    <row r="3" spans="1:37" ht="52.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>477</v>
       </c>
@@ -4692,7 +4687,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G3" s="41" t="s">
         <v>20</v>
@@ -4765,7 +4760,7 @@
       <c r="AJ3" s="39"/>
       <c r="AK3" s="39"/>
     </row>
-    <row r="4" spans="1:37" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>477</v>
       </c>
@@ -4782,7 +4777,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G4" s="41" t="s">
         <v>16</v>
@@ -4851,7 +4846,7 @@
       <c r="AJ4" s="39"/>
       <c r="AK4" s="39"/>
     </row>
-    <row r="5" spans="1:37" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
         <v>478</v>
       </c>
@@ -4868,7 +4863,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G5" s="41" t="s">
         <v>16</v>
@@ -4935,7 +4930,7 @@
       <c r="AJ5" s="39"/>
       <c r="AK5" s="39"/>
     </row>
-    <row r="6" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>477</v>
       </c>
@@ -4952,7 +4947,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G6" s="41" t="s">
         <v>20</v>
@@ -5021,7 +5016,7 @@
       <c r="AJ6" s="39"/>
       <c r="AK6" s="39"/>
     </row>
-    <row r="7" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>477</v>
       </c>
@@ -5103,7 +5098,7 @@
       <c r="AJ7" s="39"/>
       <c r="AK7" s="39"/>
     </row>
-    <row r="8" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A8" s="39" t="s">
         <v>477</v>
       </c>
@@ -5120,7 +5115,7 @@
         <v>570</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>612</v>
@@ -5202,7 +5197,7 @@
         <v>47</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G9" s="41" t="s">
         <v>48</v>
@@ -5253,13 +5248,13 @@
         <v>341</v>
       </c>
       <c r="V9" s="39" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="W9" s="39" t="s">
         <v>174</v>
       </c>
       <c r="X9" s="39" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="Y9" s="39"/>
       <c r="Z9" s="39"/>
@@ -5275,7 +5270,7 @@
       <c r="AJ9" s="39"/>
       <c r="AK9" s="39"/>
     </row>
-    <row r="10" spans="1:37" ht="52.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
         <v>477</v>
       </c>
@@ -5292,7 +5287,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G10" s="41" t="s">
         <v>20</v>
@@ -5363,12 +5358,12 @@
       <c r="AJ10" s="39"/>
       <c r="AK10" s="39"/>
     </row>
-    <row r="11" spans="1:37" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" ht="66" x14ac:dyDescent="0.3">
       <c r="A11" s="39" t="s">
         <v>477</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C11" s="39" t="s">
         <v>33</v>
@@ -5449,7 +5444,7 @@
       <c r="AJ11" s="39"/>
       <c r="AK11" s="39"/>
     </row>
-    <row r="12" spans="1:37" ht="132" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" ht="132" x14ac:dyDescent="0.3">
       <c r="A12" s="39" t="s">
         <v>477</v>
       </c>
@@ -5466,7 +5461,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="40" t="s">
@@ -5533,7 +5528,7 @@
       <c r="AJ12" s="39"/>
       <c r="AK12" s="39"/>
     </row>
-    <row r="13" spans="1:37" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" ht="66" x14ac:dyDescent="0.3">
       <c r="A13" s="39" t="s">
         <v>477</v>
       </c>
@@ -5550,7 +5545,7 @@
         <v>67</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G13" s="41"/>
       <c r="H13" s="40" t="s">
@@ -5617,7 +5612,7 @@
       <c r="AJ13" s="39"/>
       <c r="AK13" s="39"/>
     </row>
-    <row r="14" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A14" s="39" t="s">
         <v>477</v>
       </c>
@@ -5716,7 +5711,7 @@
         <v>365</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G15" s="41" t="s">
         <v>366</v>
@@ -5730,7 +5725,7 @@
       </c>
       <c r="K15" s="47">
         <f ca="1">NOW()</f>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L15" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -5750,7 +5745,7 @@
       </c>
       <c r="P15" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>19.690673503086387</v>
+        <v>19.690847071759343</v>
       </c>
       <c r="Q15" s="39" t="s">
         <v>30</v>
@@ -5801,13 +5796,13 @@
         <v>7</v>
       </c>
       <c r="F16" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G16" s="41" t="s">
         <v>20</v>
       </c>
       <c r="H16" s="40" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I16" s="41"/>
       <c r="J16" s="47">
@@ -5883,7 +5878,7 @@
         <v>367</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G17" s="41" t="s">
         <v>368</v>
@@ -5953,7 +5948,7 @@
         <v>477</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C18" s="39" t="s">
         <v>15</v>
@@ -5965,7 +5960,7 @@
         <v>373</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G18" s="41" t="s">
         <v>374</v>
@@ -6039,7 +6034,7 @@
         <v>477</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C19" s="39" t="s">
         <v>15</v>
@@ -6051,7 +6046,7 @@
         <v>34</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G19" s="41"/>
       <c r="H19" s="40" t="s">
@@ -6135,7 +6130,7 @@
         <v>90</v>
       </c>
       <c r="F20" s="51" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G20" s="41" t="s">
         <v>91</v>
@@ -6221,7 +6216,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G21" s="41" t="s">
         <v>17</v>
@@ -6237,7 +6232,7 @@
       </c>
       <c r="K21" s="47">
         <f ca="1">NOW()</f>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L21" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -6257,7 +6252,7 @@
       </c>
       <c r="P21" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>24.124006836419721</v>
+        <v>24.124180405092677</v>
       </c>
       <c r="Q21" s="39" t="s">
         <v>30</v>
@@ -6308,7 +6303,7 @@
         <v>26</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G22" s="41" t="s">
         <v>27</v>
@@ -6394,7 +6389,7 @@
         <v>95</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G23" s="41" t="s">
         <v>96</v>
@@ -6478,7 +6473,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G24" s="41" t="s">
         <v>17</v>
@@ -6565,10 +6560,10 @@
         <v>45</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F25" s="51" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G25" s="41" t="s">
         <v>426</v>
@@ -6654,7 +6649,7 @@
         <v>104</v>
       </c>
       <c r="F26" s="51" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G26" s="41"/>
       <c r="H26" s="40" t="s">
@@ -6736,7 +6731,7 @@
         <v>105</v>
       </c>
       <c r="F27" s="51" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G27" s="41" t="s">
         <v>106</v>
@@ -6820,7 +6815,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G28" s="41" t="s">
         <v>20</v>
@@ -6902,7 +6897,7 @@
         <v>7</v>
       </c>
       <c r="F29" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G29" s="41" t="s">
         <v>20</v>
@@ -6984,7 +6979,7 @@
         <v>109</v>
       </c>
       <c r="F30" s="51" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G30" s="41" t="s">
         <v>110</v>
@@ -7066,7 +7061,7 @@
         <v>13</v>
       </c>
       <c r="F31" s="51" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G31" s="41" t="s">
         <v>18</v>
@@ -7082,7 +7077,7 @@
       </c>
       <c r="K31" s="47">
         <f t="shared" ref="K31:K37" ca="1" si="1">NOW()</f>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L31" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -7102,7 +7097,7 @@
       </c>
       <c r="P31" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>16.690673503086387</v>
+        <v>16.690847071759343</v>
       </c>
       <c r="Q31" s="39" t="s">
         <v>30</v>
@@ -7151,7 +7146,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="51" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G32" s="41" t="s">
         <v>17</v>
@@ -7167,7 +7162,7 @@
       </c>
       <c r="K32" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L32" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -7187,7 +7182,7 @@
       </c>
       <c r="P32" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4567676851851825</v>
+        <v>2.4567819511035078</v>
       </c>
       <c r="Q32" s="39" t="s">
         <v>31</v>
@@ -7236,7 +7231,7 @@
         <v>120</v>
       </c>
       <c r="F33" s="51" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G33" s="41"/>
       <c r="H33" s="40" t="s">
@@ -7250,7 +7245,7 @@
       </c>
       <c r="K33" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L33" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -7270,7 +7265,7 @@
       </c>
       <c r="P33" s="42">
         <f t="shared" ref="P33:P64" ca="1" si="2">IF((Q33="Days"),((K33-J33+1)),IF(Q33="Months",((K33-J33)/30),((K33-J33)/365)))</f>
-        <v>32.89067350308639</v>
+        <v>32.890847071759346</v>
       </c>
       <c r="Q33" s="39" t="s">
         <v>30</v>
@@ -7319,7 +7314,7 @@
         <v>131</v>
       </c>
       <c r="F34" s="51" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G34" s="41"/>
       <c r="H34" s="40" t="s">
@@ -7333,7 +7328,7 @@
       </c>
       <c r="K34" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L34" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -7353,7 +7348,7 @@
       </c>
       <c r="P34" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>35.957340169753053</v>
+        <v>35.957513738426009</v>
       </c>
       <c r="Q34" s="39" t="s">
         <v>30</v>
@@ -7399,10 +7394,10 @@
         <v>115</v>
       </c>
       <c r="E35" s="40" t="s">
+        <v>655</v>
+      </c>
+      <c r="F35" s="51" t="s">
         <v>656</v>
-      </c>
-      <c r="F35" s="51" t="s">
-        <v>657</v>
       </c>
       <c r="G35" s="41"/>
       <c r="H35" s="40" t="s">
@@ -7416,7 +7411,7 @@
       </c>
       <c r="K35" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L35" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -7436,7 +7431,7 @@
       </c>
       <c r="P35" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>23.957340169753056</v>
+        <v>23.957513738426012</v>
       </c>
       <c r="Q35" s="39" t="s">
         <v>30</v>
@@ -7485,7 +7480,7 @@
         <v>121</v>
       </c>
       <c r="F36" s="51" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G36" s="41" t="s">
         <v>122</v>
@@ -7501,7 +7496,7 @@
       </c>
       <c r="K36" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L36" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -7521,7 +7516,7 @@
       </c>
       <c r="P36" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>33.924006836419721</v>
+        <v>33.924180405092677</v>
       </c>
       <c r="Q36" s="39" t="s">
         <v>30</v>
@@ -7570,7 +7565,7 @@
         <v>129</v>
       </c>
       <c r="F37" s="51" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G37" s="41" t="s">
         <v>381</v>
@@ -7584,7 +7579,7 @@
       </c>
       <c r="K37" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L37" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -7604,7 +7599,7 @@
       </c>
       <c r="P37" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>35.957340169753053</v>
+        <v>35.957513738426009</v>
       </c>
       <c r="Q37" s="39" t="s">
         <v>30</v>
@@ -7653,7 +7648,7 @@
         <v>47</v>
       </c>
       <c r="F38" s="51" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G38" s="41" t="s">
         <v>48</v>
@@ -7737,7 +7732,7 @@
         <v>618</v>
       </c>
       <c r="F39" s="51" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G39" s="41" t="s">
         <v>619</v>
@@ -7821,7 +7816,7 @@
         <v>7</v>
       </c>
       <c r="F40" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G40" s="41" t="s">
         <v>20</v>
@@ -7903,7 +7898,7 @@
         <v>620</v>
       </c>
       <c r="F41" s="51" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G41" s="41" t="s">
         <v>615</v>
@@ -7987,7 +7982,7 @@
         <v>67</v>
       </c>
       <c r="F42" s="51" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G42" s="41"/>
       <c r="H42" s="40" t="s">
@@ -8050,7 +8045,7 @@
       <c r="AJ42" s="39"/>
       <c r="AK42" s="39"/>
     </row>
-    <row r="43" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A43" s="39" t="s">
         <v>477</v>
       </c>
@@ -8058,7 +8053,7 @@
         <v>155</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D43" s="39" t="s">
         <v>401</v>
@@ -8067,7 +8062,7 @@
         <v>6</v>
       </c>
       <c r="F43" s="51" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G43" s="41" t="s">
         <v>16</v>
@@ -8132,7 +8127,7 @@
       <c r="AJ43" s="39"/>
       <c r="AK43" s="39"/>
     </row>
-    <row r="44" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A44" s="39" t="s">
         <v>477</v>
       </c>
@@ -8140,7 +8135,7 @@
         <v>155</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D44" s="39" t="s">
         <v>401</v>
@@ -8149,7 +8144,7 @@
         <v>6</v>
       </c>
       <c r="F44" s="51" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G44" s="41" t="s">
         <v>16</v>
@@ -8214,7 +8209,7 @@
       <c r="AJ44" s="39"/>
       <c r="AK44" s="39"/>
     </row>
-    <row r="45" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A45" s="39" t="s">
         <v>477</v>
       </c>
@@ -8222,7 +8217,7 @@
         <v>155</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D45" s="39" t="s">
         <v>401</v>
@@ -8231,7 +8226,7 @@
         <v>536</v>
       </c>
       <c r="F45" s="51" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G45" s="41"/>
       <c r="H45" s="40" t="s">
@@ -8294,7 +8289,7 @@
       <c r="AJ45" s="39"/>
       <c r="AK45" s="39"/>
     </row>
-    <row r="46" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:37" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A46" s="39" t="s">
         <v>477</v>
       </c>
@@ -8302,7 +8297,7 @@
         <v>155</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D46" s="39" t="s">
         <v>401</v>
@@ -8311,11 +8306,11 @@
         <v>7</v>
       </c>
       <c r="F46" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G46" s="41"/>
       <c r="H46" s="40" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I46" s="41"/>
       <c r="J46" s="48"/>
@@ -8349,13 +8344,13 @@
       <c r="W46" s="39"/>
       <c r="X46" s="39"/>
       <c r="Y46" s="39" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="Z46" s="39" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AA46" s="39" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AB46" s="39"/>
       <c r="AC46" s="39"/>
@@ -8376,7 +8371,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D47" s="39" t="s">
         <v>33</v>
@@ -8385,13 +8380,13 @@
         <v>47</v>
       </c>
       <c r="F47" s="51" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G47" s="41" t="s">
         <v>48</v>
       </c>
       <c r="H47" s="40" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="I47" s="41" t="s">
         <v>423</v>
@@ -8458,7 +8453,7 @@
       <c r="AJ47" s="39"/>
       <c r="AK47" s="39"/>
     </row>
-    <row r="48" spans="1:37" ht="52.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:37" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A48" s="39" t="s">
         <v>477</v>
       </c>
@@ -8466,13 +8461,13 @@
         <v>46</v>
       </c>
       <c r="C48" s="39" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D48" s="39" t="s">
         <v>397</v>
       </c>
       <c r="E48" s="40" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F48" s="40"/>
       <c r="G48" s="41"/>
@@ -8523,13 +8518,13 @@
       <c r="W48" s="39"/>
       <c r="X48" s="39"/>
       <c r="Y48" s="39" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="Z48" s="39" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AA48" s="39" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AB48" s="39"/>
       <c r="AC48" s="39"/>
@@ -8542,7 +8537,7 @@
       <c r="AJ48" s="39"/>
       <c r="AK48" s="39"/>
     </row>
-    <row r="49" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:37" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A49" s="39" t="s">
         <v>478</v>
       </c>
@@ -8559,7 +8554,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G49" s="41" t="s">
         <v>20</v>
@@ -8624,7 +8619,7 @@
       <c r="AJ49" s="39"/>
       <c r="AK49" s="39"/>
     </row>
-    <row r="50" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A50" s="39" t="s">
         <v>478</v>
       </c>
@@ -8641,7 +8636,7 @@
         <v>536</v>
       </c>
       <c r="F50" s="51" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G50" s="41"/>
       <c r="H50" s="40" t="s">
@@ -8704,7 +8699,7 @@
       <c r="AJ50" s="39"/>
       <c r="AK50" s="39"/>
     </row>
-    <row r="51" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
         <v>478</v>
       </c>
@@ -8721,7 +8716,7 @@
         <v>371</v>
       </c>
       <c r="F51" s="51" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G51" s="41"/>
       <c r="H51" s="40" t="s">
@@ -8784,7 +8779,7 @@
       <c r="AJ51" s="39"/>
       <c r="AK51" s="39"/>
     </row>
-    <row r="52" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A52" s="39" t="s">
         <v>478</v>
       </c>
@@ -8801,7 +8796,7 @@
         <v>135</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G52" s="41" t="s">
         <v>136</v>
@@ -8868,7 +8863,7 @@
       <c r="AJ52" s="39"/>
       <c r="AK52" s="39"/>
     </row>
-    <row r="53" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:37" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A53" s="39" t="s">
         <v>478</v>
       </c>
@@ -8885,7 +8880,7 @@
         <v>144</v>
       </c>
       <c r="F53" s="51" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G53" s="41"/>
       <c r="H53" s="40" t="s">
@@ -8948,7 +8943,7 @@
       <c r="AJ53" s="39"/>
       <c r="AK53" s="39"/>
     </row>
-    <row r="54" spans="1:37" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:37" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="39" t="s">
         <v>478</v>
       </c>
@@ -8965,7 +8960,7 @@
         <v>345</v>
       </c>
       <c r="F54" s="51" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G54" s="41" t="s">
         <v>347</v>
@@ -9022,7 +9017,7 @@
       <c r="AJ54" s="39"/>
       <c r="AK54" s="39"/>
     </row>
-    <row r="55" spans="1:37" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:37" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="39" t="s">
         <v>478</v>
       </c>
@@ -9039,7 +9034,7 @@
         <v>537</v>
       </c>
       <c r="F55" s="51" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G55" s="41"/>
       <c r="H55" s="40" t="s">
@@ -9098,7 +9093,7 @@
       <c r="AJ55" s="39"/>
       <c r="AK55" s="39"/>
     </row>
-    <row r="56" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:37" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A56" s="39" t="s">
         <v>478</v>
       </c>
@@ -9115,7 +9110,7 @@
         <v>7</v>
       </c>
       <c r="F56" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G56" s="41" t="s">
         <v>20</v>
@@ -9180,7 +9175,7 @@
       <c r="AJ56" s="39"/>
       <c r="AK56" s="39"/>
     </row>
-    <row r="57" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:37" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A57" s="39" t="s">
         <v>478</v>
       </c>
@@ -9197,7 +9192,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G57" s="41" t="s">
         <v>20</v>
@@ -9264,7 +9259,7 @@
       <c r="AJ57" s="39"/>
       <c r="AK57" s="39"/>
     </row>
-    <row r="58" spans="1:37" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:37" ht="66" x14ac:dyDescent="0.3">
       <c r="A58" s="39" t="s">
         <v>478</v>
       </c>
@@ -9281,7 +9276,7 @@
         <v>7</v>
       </c>
       <c r="F58" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G58" s="41" t="s">
         <v>20</v>
@@ -9348,12 +9343,12 @@
       <c r="AJ58" s="39"/>
       <c r="AK58" s="39"/>
     </row>
-    <row r="59" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A59" s="39" t="s">
         <v>478</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C59" s="39" t="s">
         <v>33</v>
@@ -9443,13 +9438,13 @@
         <v>7</v>
       </c>
       <c r="F60" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G60" s="41" t="s">
         <v>20</v>
       </c>
       <c r="H60" s="40" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I60" s="41"/>
       <c r="J60" s="47">
@@ -9525,7 +9520,7 @@
         <v>36</v>
       </c>
       <c r="F61" s="51" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G61" s="41" t="s">
         <v>37</v>
@@ -9605,7 +9600,7 @@
         <v>11</v>
       </c>
       <c r="F62" s="51" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G62" s="41" t="s">
         <v>17</v>
@@ -9685,7 +9680,7 @@
         <v>85</v>
       </c>
       <c r="F63" s="51" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G63" s="41" t="s">
         <v>86</v>
@@ -9767,7 +9762,7 @@
         <v>7</v>
       </c>
       <c r="F64" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G64" s="41" t="s">
         <v>20</v>
@@ -9837,7 +9832,7 @@
         <v>478</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C65" s="39" t="s">
         <v>388</v>
@@ -9849,7 +9844,7 @@
         <v>139</v>
       </c>
       <c r="F65" s="51" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G65" s="41"/>
       <c r="H65" s="40" t="s">
@@ -9929,7 +9924,7 @@
         <v>149</v>
       </c>
       <c r="F66" s="51" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="G66" s="41"/>
       <c r="H66" s="40" t="s">
@@ -10011,7 +10006,7 @@
         <v>139</v>
       </c>
       <c r="F67" s="51" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G67" s="41"/>
       <c r="H67" s="40" t="s">
@@ -10025,7 +10020,7 @@
       </c>
       <c r="K67" s="47">
         <f ca="1">NOW()</f>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L67" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -10045,7 +10040,7 @@
       </c>
       <c r="P67" s="42">
         <f t="shared" ca="1" si="3"/>
-        <v>28.890673503086386</v>
+        <v>28.890847071759346</v>
       </c>
       <c r="Q67" s="39" t="s">
         <v>30</v>
@@ -10094,7 +10089,7 @@
         <v>147</v>
       </c>
       <c r="F68" s="51" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G68" s="41"/>
       <c r="H68" s="40" t="s">
@@ -10106,7 +10101,7 @@
       </c>
       <c r="K68" s="47">
         <f ca="1">NOW()</f>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L68" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -10126,7 +10121,7 @@
       </c>
       <c r="P68" s="42">
         <f t="shared" ca="1" si="3"/>
-        <v>9.210192342719429</v>
+        <v>9.2102066086377548</v>
       </c>
       <c r="Q68" s="39" t="s">
         <v>31</v>
@@ -10175,7 +10170,7 @@
         <v>127</v>
       </c>
       <c r="F69" s="51" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G69" s="41" t="s">
         <v>126</v>
@@ -10189,7 +10184,7 @@
       </c>
       <c r="K69" s="47">
         <f ca="1">NOW()</f>
-        <v>44452.720205092592</v>
+        <v>44452.72541215278</v>
       </c>
       <c r="L69" s="49">
         <f>MONTH(cv.table[[#This Row],[Start]])</f>
@@ -10209,7 +10204,7 @@
       </c>
       <c r="P69" s="42">
         <f t="shared" ca="1" si="3"/>
-        <v>35.957340169753053</v>
+        <v>35.957513738426009</v>
       </c>
       <c r="Q69" s="39" t="s">
         <v>30</v>
@@ -10244,30 +10239,30 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="L62:O62 K63:O64 K67:O67 K69:O1048576 K1:O61">
-    <cfRule type="timePeriod" dxfId="14" priority="9" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="86" priority="9" timePeriod="today">
       <formula>FLOOR(K1,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="timePeriod" dxfId="13" priority="5" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="85" priority="5" timePeriod="today">
       <formula>FLOOR(K62,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65:O66">
-    <cfRule type="timePeriod" dxfId="12" priority="4" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="84" priority="4" timePeriod="today">
       <formula>FLOOR(K65,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:O68">
-    <cfRule type="timePeriod" dxfId="11" priority="3" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="83" priority="3" timePeriod="today">
       <formula>FLOOR(K68,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:AK69">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="82" priority="1">
       <formula>$A2="Disclude"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="81" priority="2">
       <formula>$A2="Include"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12218,31 +12213,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A49">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"Offered"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"Interview"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"Applied"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"Offered-Declined"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"Offered-Accepted"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"Interview-Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
       <formula>"No response"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12330,7 +12325,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>9</v>
@@ -12557,7 +12552,7 @@
         <v>155</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>400</v>

</xml_diff>